<commit_message>
updated styling and homepage layout
</commit_message>
<xml_diff>
--- a/matrix.xlsx
+++ b/matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5920" yWindow="0" windowWidth="17800" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="24040" windowHeight="15300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>HTML</t>
   </si>
@@ -82,6 +82,45 @@
   </si>
   <si>
     <t>Mongo</t>
+  </si>
+  <si>
+    <t>Matrix for JSON file</t>
+  </si>
+  <si>
+    <t>Text of Matrix formula</t>
+  </si>
+  <si>
+    <t>checking MATRIX #s:</t>
+  </si>
+  <si>
+    <t>Checking Matrix #s</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,0,0,0,0,0,0,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,0,0,0,0,0,0,0,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,0,0,0,0,0,0,0,0,1,0]</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,0,0,0,0,0,0,1,0,0,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,0,0,0,0,0,0,0,1,0,0]</t>
+  </si>
+  <si>
+    <t>[1,1,1,0,0,0,1,0,0,0,0,0,0,0]</t>
+  </si>
+  <si>
+    <t>[1,1,1,1,1,0,0,1,0,0,0,0,0,0]</t>
+  </si>
+  <si>
+    <t>[1,1,1,1,1,1,0,0,1,1,0,0,0,0]</t>
+  </si>
+  <si>
+    <t>[1,1,1,1,1,0,1,0,0,0,0,0,0,0]</t>
   </si>
 </sst>
 </file>
@@ -130,8 +169,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -192,7 +265,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -221,6 +294,23 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -249,6 +339,23 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -578,14 +685,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:O30"/>
+  <dimension ref="A4:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
@@ -599,7 +707,7 @@
     <col min="12" max="13" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:23">
       <c r="C4" t="s">
         <v>10</v>
       </c>
@@ -610,57 +718,69 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="15" spans="1:23">
+      <c r="Q15">
+        <f>SUM(Q16:Q26)</f>
+        <v>24</v>
+      </c>
+      <c r="S15" t="s">
+        <v>21</v>
+      </c>
+      <c r="W15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -703,8 +823,11 @@
       <c r="O16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="Q16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -750,8 +873,19 @@
       <c r="O17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="Q17">
+        <f>SUM(B17:O17)</f>
+        <v>4</v>
+      </c>
+      <c r="S17" t="str">
+        <f>"["&amp;B17&amp;","&amp;C17&amp;","&amp;D17&amp;","&amp;E17&amp;","&amp;F17&amp;","&amp;G17&amp;","&amp;H17&amp;","&amp;I17&amp;","&amp;J17&amp;","&amp;K17&amp;","&amp;L17&amp;","&amp;M17&amp;","&amp;N17&amp;","&amp;O17&amp;"]"</f>
+        <v>[0,0,0,0,0,0,0,0,0,0,1,1,1,1]</v>
+      </c>
+      <c r="W17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -797,8 +931,19 @@
       <c r="O18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="Q18">
+        <f>SUM(B18:O18)</f>
+        <v>4</v>
+      </c>
+      <c r="S18" t="str">
+        <f t="shared" ref="S18:S30" si="0">"["&amp;B18&amp;","&amp;C18&amp;","&amp;D18&amp;","&amp;E18&amp;","&amp;F18&amp;","&amp;G18&amp;","&amp;H18&amp;","&amp;I18&amp;","&amp;J18&amp;","&amp;K18&amp;","&amp;L18&amp;","&amp;M18&amp;","&amp;N18&amp;","&amp;O18&amp;"]"</f>
+        <v>[0,0,0,0,0,0,0,0,0,0,1,1,1,1]</v>
+      </c>
+      <c r="W18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -844,8 +989,19 @@
       <c r="O19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="Q19">
+        <f>SUM(B19:O19)</f>
+        <v>4</v>
+      </c>
+      <c r="S19" t="str">
+        <f t="shared" si="0"/>
+        <v>[0,0,0,0,0,0,0,0,0,0,1,1,1,1]</v>
+      </c>
+      <c r="W19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -891,8 +1047,19 @@
       <c r="O20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="Q20">
+        <f>SUM(B20:O20)</f>
+        <v>3</v>
+      </c>
+      <c r="S20" t="str">
+        <f t="shared" si="0"/>
+        <v>[0,0,0,0,0,0,0,0,0,0,0,1,1,1]</v>
+      </c>
+      <c r="W20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -938,8 +1105,19 @@
       <c r="O21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="Q21">
+        <f>SUM(B21:O21)</f>
+        <v>3</v>
+      </c>
+      <c r="S21" t="str">
+        <f t="shared" si="0"/>
+        <v>[0,0,0,0,0,0,0,0,0,0,0,1,1,1]</v>
+      </c>
+      <c r="W21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -985,8 +1163,19 @@
       <c r="O22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="Q22">
+        <f>SUM(B22:O22)</f>
+        <v>1</v>
+      </c>
+      <c r="S22" t="str">
+        <f t="shared" si="0"/>
+        <v>[0,0,0,0,0,0,0,0,0,0,0,0,1,0]</v>
+      </c>
+      <c r="W22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1032,8 +1221,19 @@
       <c r="O23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="Q23">
+        <f>SUM(B23:O23)</f>
+        <v>2</v>
+      </c>
+      <c r="S23" t="str">
+        <f t="shared" si="0"/>
+        <v>[0,0,0,0,0,0,0,0,0,0,1,0,0,1]</v>
+      </c>
+      <c r="W23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1079,8 +1279,19 @@
       <c r="O24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="Q24">
+        <f>SUM(B24:O24)</f>
+        <v>1</v>
+      </c>
+      <c r="S24" t="str">
+        <f t="shared" si="0"/>
+        <v>[0,0,0,0,0,0,0,0,0,0,0,1,0,0]</v>
+      </c>
+      <c r="W24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1126,8 +1337,19 @@
       <c r="O25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="Q25">
+        <f>SUM(B25:O25)</f>
+        <v>1</v>
+      </c>
+      <c r="S25" t="str">
+        <f t="shared" si="0"/>
+        <v>[0,0,0,0,0,0,0,0,0,0,0,0,1,0]</v>
+      </c>
+      <c r="W25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1173,8 +1395,19 @@
       <c r="O26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="Q26">
+        <f>SUM(B26:O26)</f>
+        <v>1</v>
+      </c>
+      <c r="S26" t="str">
+        <f t="shared" si="0"/>
+        <v>[0,0,0,0,0,0,0,0,0,0,0,0,1,0]</v>
+      </c>
+      <c r="W26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1209,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -1220,8 +1453,15 @@
       <c r="O27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="S27" t="str">
+        <f t="shared" si="0"/>
+        <v>[1,1,1,0,0,0,1,0,0,0,0,0,0,0]</v>
+      </c>
+      <c r="W27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1259,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -1267,8 +1507,15 @@
       <c r="O28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="S28" t="str">
+        <f t="shared" si="0"/>
+        <v>[1,1,1,1,1,0,0,1,0,0,0,0,0,0]</v>
+      </c>
+      <c r="W28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1309,13 +1556,20 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="S29" t="str">
+        <f t="shared" si="0"/>
+        <v>[1,1,1,1,1,1,0,0,1,1,0,0,0,0]</v>
+      </c>
+      <c r="W29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1359,7 +1613,77 @@
         <v>0</v>
       </c>
       <c r="O30">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="S30" t="str">
+        <f t="shared" si="0"/>
+        <v>[1,1,1,1,1,0,1,0,0,0,0,0,0,0]</v>
+      </c>
+      <c r="W30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32">
+        <f>SUM(B17:B30)</f>
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <f>SUM(C17:C30)</f>
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <f>SUM(D17:D30)</f>
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <f>SUM(E17:E30)</f>
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <f>SUM(F17:F30)</f>
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <f>SUM(G17:G30)</f>
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <f>SUM(H17:H30)</f>
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <f>SUM(I17:I30)</f>
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <f>SUM(J17:J30)</f>
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <f>SUM(K17:K30)</f>
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33">
+        <f>SUM(B32:K32)</f>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to be responsive
</commit_message>
<xml_diff>
--- a/matrix.xlsx
+++ b/matrix.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="24040" windowHeight="15300" tabRatio="500"/>
+    <workbookView xWindow="6340" yWindow="0" windowWidth="17680" windowHeight="15300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Colors" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="52">
   <si>
     <t>HTML</t>
   </si>
@@ -121,6 +122,60 @@
   </si>
   <si>
     <t>[1,1,1,1,1,0,1,0,0,0,0,0,0,0]</t>
+  </si>
+  <si>
+    <t>#708090</t>
+  </si>
+  <si>
+    <t>#6093BF</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>#3C74A6</t>
+  </si>
+  <si>
+    <t>#194973</t>
+  </si>
+  <si>
+    <t>#FF8200</t>
+  </si>
+  <si>
+    <t>#F09F0D</t>
+  </si>
+  <si>
+    <t>#C73C1C</t>
+  </si>
+  <si>
+    <t>#5F9EA0</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>#66CDAA</t>
+  </si>
+  <si>
+    <t>#D8BFD8</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>#4B0082</t>
+  </si>
+  <si>
+    <t>color array for JS</t>
+  </si>
+  <si>
+    <t>array for skills</t>
   </si>
 </sst>
 </file>
@@ -169,8 +224,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -265,7 +362,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="133">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -311,6 +408,27 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -356,6 +474,27 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -687,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -698,13 +837,13 @@
     <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.33203125" customWidth="1"/>
-    <col min="8" max="8" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:23">
@@ -794,19 +933,19 @@
         <v>13</v>
       </c>
       <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s">
         <v>5</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>20</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>6</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>7</v>
-      </c>
-      <c r="J16" t="s">
-        <v>8</v>
       </c>
       <c r="K16" t="s">
         <v>9</v>
@@ -878,7 +1017,7 @@
         <v>4</v>
       </c>
       <c r="S17" t="str">
-        <f>"["&amp;B17&amp;","&amp;C17&amp;","&amp;D17&amp;","&amp;E17&amp;","&amp;F17&amp;","&amp;G17&amp;","&amp;H17&amp;","&amp;I17&amp;","&amp;J17&amp;","&amp;K17&amp;","&amp;L17&amp;","&amp;M17&amp;","&amp;N17&amp;","&amp;O17&amp;"]"</f>
+        <f>"["&amp;B17&amp;","&amp;C17&amp;","&amp;D17&amp;","&amp;E17&amp;","&amp;G17&amp;","&amp;H17&amp;","&amp;I17&amp;","&amp;J17&amp;","&amp;F17&amp;","&amp;K17&amp;","&amp;L17&amp;","&amp;M17&amp;","&amp;N17&amp;","&amp;O17&amp;"]"</f>
         <v>[0,0,0,0,0,0,0,0,0,0,1,1,1,1]</v>
       </c>
       <c r="W17" t="s">
@@ -936,7 +1075,7 @@
         <v>4</v>
       </c>
       <c r="S18" t="str">
-        <f t="shared" ref="S18:S30" si="0">"["&amp;B18&amp;","&amp;C18&amp;","&amp;D18&amp;","&amp;E18&amp;","&amp;F18&amp;","&amp;G18&amp;","&amp;H18&amp;","&amp;I18&amp;","&amp;J18&amp;","&amp;K18&amp;","&amp;L18&amp;","&amp;M18&amp;","&amp;N18&amp;","&amp;O18&amp;"]"</f>
+        <f>"["&amp;B18&amp;","&amp;C18&amp;","&amp;D18&amp;","&amp;E18&amp;","&amp;G18&amp;","&amp;H18&amp;","&amp;I18&amp;","&amp;J18&amp;","&amp;F18&amp;","&amp;K18&amp;","&amp;L18&amp;","&amp;M18&amp;","&amp;N18&amp;","&amp;O18&amp;"]"</f>
         <v>[0,0,0,0,0,0,0,0,0,0,1,1,1,1]</v>
       </c>
       <c r="W18" t="s">
@@ -994,7 +1133,7 @@
         <v>4</v>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="0"/>
+        <f>"["&amp;B19&amp;","&amp;C19&amp;","&amp;D19&amp;","&amp;E19&amp;","&amp;G19&amp;","&amp;H19&amp;","&amp;I19&amp;","&amp;J19&amp;","&amp;F19&amp;","&amp;K19&amp;","&amp;L19&amp;","&amp;M19&amp;","&amp;N19&amp;","&amp;O19&amp;"]"</f>
         <v>[0,0,0,0,0,0,0,0,0,0,1,1,1,1]</v>
       </c>
       <c r="W19" t="s">
@@ -1052,7 +1191,7 @@
         <v>3</v>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="0"/>
+        <f>"["&amp;B20&amp;","&amp;C20&amp;","&amp;D20&amp;","&amp;E20&amp;","&amp;G20&amp;","&amp;H20&amp;","&amp;I20&amp;","&amp;J20&amp;","&amp;F20&amp;","&amp;K20&amp;","&amp;L20&amp;","&amp;M20&amp;","&amp;N20&amp;","&amp;O20&amp;"]"</f>
         <v>[0,0,0,0,0,0,0,0,0,0,0,1,1,1]</v>
       </c>
       <c r="W20" t="s">
@@ -1061,7 +1200,7 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1097,29 +1236,29 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21">
         <v>1</v>
       </c>
       <c r="O21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q21">
         <f>SUM(B21:O21)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" si="0"/>
-        <v>[0,0,0,0,0,0,0,0,0,0,0,1,1,1]</v>
+        <f>"["&amp;B21&amp;","&amp;C21&amp;","&amp;D21&amp;","&amp;E21&amp;","&amp;G21&amp;","&amp;H21&amp;","&amp;I21&amp;","&amp;J21&amp;","&amp;F21&amp;","&amp;K21&amp;","&amp;L21&amp;","&amp;M21&amp;","&amp;N21&amp;","&amp;O21&amp;"]"</f>
+        <v>[0,0,0,0,0,0,0,0,0,0,0,0,1,0]</v>
       </c>
       <c r="W21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1155,29 +1294,29 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22">
         <v>1</v>
       </c>
       <c r="O22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22">
         <f>SUM(B22:O22)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S22" t="str">
-        <f t="shared" si="0"/>
-        <v>[0,0,0,0,0,0,0,0,0,0,0,0,1,0]</v>
+        <f>"["&amp;B22&amp;","&amp;C22&amp;","&amp;D22&amp;","&amp;E22&amp;","&amp;G22&amp;","&amp;H22&amp;","&amp;I22&amp;","&amp;J22&amp;","&amp;F22&amp;","&amp;K22&amp;","&amp;L22&amp;","&amp;M22&amp;","&amp;N22&amp;","&amp;O22&amp;"]"</f>
+        <v>[0,0,0,0,0,0,0,0,0,0,0,1,1,1]</v>
       </c>
       <c r="W22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1210,32 +1349,32 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q23">
         <f>SUM(B23:O23)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S23" t="str">
-        <f t="shared" si="0"/>
-        <v>[0,0,0,0,0,0,0,0,0,0,1,0,0,1]</v>
+        <f>"["&amp;B23&amp;","&amp;C23&amp;","&amp;D23&amp;","&amp;E23&amp;","&amp;G23&amp;","&amp;H23&amp;","&amp;I23&amp;","&amp;J23&amp;","&amp;F23&amp;","&amp;K23&amp;","&amp;L23&amp;","&amp;M23&amp;","&amp;N23&amp;","&amp;O23&amp;"]"</f>
+        <v>[0,0,0,0,0,0,0,0,0,0,0,0,1,0]</v>
       </c>
       <c r="W23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1268,32 +1407,32 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24">
         <v>0</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24">
         <f>SUM(B24:O24)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="0"/>
-        <v>[0,0,0,0,0,0,0,0,0,0,0,1,0,0]</v>
+        <f>"["&amp;B24&amp;","&amp;C24&amp;","&amp;D24&amp;","&amp;E24&amp;","&amp;G24&amp;","&amp;H24&amp;","&amp;I24&amp;","&amp;J24&amp;","&amp;F24&amp;","&amp;K24&amp;","&amp;L24&amp;","&amp;M24&amp;","&amp;N24&amp;","&amp;O24&amp;"]"</f>
+        <v>[0,0,0,0,0,0,0,0,0,0,1,0,0,1]</v>
       </c>
       <c r="W24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1329,10 +1468,10 @@
         <v>0</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1342,11 +1481,11 @@
         <v>1</v>
       </c>
       <c r="S25" t="str">
-        <f t="shared" si="0"/>
-        <v>[0,0,0,0,0,0,0,0,0,0,0,0,1,0]</v>
+        <f>"["&amp;B25&amp;","&amp;C25&amp;","&amp;D25&amp;","&amp;E25&amp;","&amp;G25&amp;","&amp;H25&amp;","&amp;I25&amp;","&amp;J25&amp;","&amp;F25&amp;","&amp;K25&amp;","&amp;L25&amp;","&amp;M25&amp;","&amp;N25&amp;","&amp;O25&amp;"]"</f>
+        <v>[0,0,0,0,0,0,0,0,0,0,0,1,0,0]</v>
       </c>
       <c r="W25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:23">
@@ -1400,7 +1539,7 @@
         <v>1</v>
       </c>
       <c r="S26" t="str">
-        <f t="shared" si="0"/>
+        <f>"["&amp;B26&amp;","&amp;C26&amp;","&amp;D26&amp;","&amp;E26&amp;","&amp;G26&amp;","&amp;H26&amp;","&amp;I26&amp;","&amp;J26&amp;","&amp;F26&amp;","&amp;K26&amp;","&amp;L26&amp;","&amp;M26&amp;","&amp;N26&amp;","&amp;O26&amp;"]"</f>
         <v>[0,0,0,0,0,0,0,0,0,0,0,0,1,0]</v>
       </c>
       <c r="W26" t="s">
@@ -1430,10 +1569,10 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -1454,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="S27" t="str">
-        <f t="shared" si="0"/>
+        <f>"["&amp;B27&amp;","&amp;C27&amp;","&amp;D27&amp;","&amp;E27&amp;","&amp;G27&amp;","&amp;H27&amp;","&amp;I27&amp;","&amp;J27&amp;","&amp;F27&amp;","&amp;K27&amp;","&amp;L27&amp;","&amp;M27&amp;","&amp;N27&amp;","&amp;O27&amp;"]"</f>
         <v>[1,1,1,0,0,0,1,0,0,0,0,0,0,0]</v>
       </c>
       <c r="W27" t="s">
@@ -1478,19 +1617,19 @@
         <v>1</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -1508,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="S28" t="str">
-        <f t="shared" si="0"/>
+        <f>"["&amp;B28&amp;","&amp;C28&amp;","&amp;D28&amp;","&amp;E28&amp;","&amp;G28&amp;","&amp;H28&amp;","&amp;I28&amp;","&amp;J28&amp;","&amp;F28&amp;","&amp;K28&amp;","&amp;L28&amp;","&amp;M28&amp;","&amp;N28&amp;","&amp;O28&amp;"]"</f>
         <v>[1,1,1,1,1,0,0,1,0,0,0,0,0,0]</v>
       </c>
       <c r="W28" t="s">
@@ -1538,13 +1677,13 @@
         <v>1</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <v>0</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -1562,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="S29" t="str">
-        <f t="shared" si="0"/>
+        <f>"["&amp;B29&amp;","&amp;C29&amp;","&amp;D29&amp;","&amp;E29&amp;","&amp;G29&amp;","&amp;H29&amp;","&amp;I29&amp;","&amp;J29&amp;","&amp;F29&amp;","&amp;K29&amp;","&amp;L29&amp;","&amp;M29&amp;","&amp;N29&amp;","&amp;O29&amp;"]"</f>
         <v>[1,1,1,1,1,1,0,0,1,1,0,0,0,0]</v>
       </c>
       <c r="W29" t="s">
@@ -1586,16 +1725,16 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -1616,7 +1755,7 @@
         <v>0</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" si="0"/>
+        <f>"["&amp;B30&amp;","&amp;C30&amp;","&amp;D30&amp;","&amp;E30&amp;","&amp;G30&amp;","&amp;H30&amp;","&amp;I30&amp;","&amp;J30&amp;","&amp;F30&amp;","&amp;K30&amp;","&amp;L30&amp;","&amp;M30&amp;","&amp;N30&amp;","&amp;O30&amp;"]"</f>
         <v>[1,1,1,1,1,0,1,0,0,0,0,0,0,0]</v>
       </c>
       <c r="W30" t="s">
@@ -1645,19 +1784,19 @@
       </c>
       <c r="F32">
         <f>SUM(F17:F30)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <f>SUM(G17:G30)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H32">
         <f>SUM(H17:H30)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <f>SUM(I17:I30)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J32">
         <f>SUM(J17:J30)</f>
@@ -1684,6 +1823,371 @@
       <c r="A33">
         <f>SUM(B32:K32)</f>
         <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="str">
+        <f>"'"&amp;C3&amp;"'"&amp;","</f>
+        <v>'#6093BF',</v>
+      </c>
+      <c r="F3" t="str">
+        <f>"'"&amp;B3&amp;"'"&amp;","</f>
+        <v>'HTML',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D15" si="0">"'"&amp;C4&amp;"'"&amp;","</f>
+        <v>'#3C74A6',</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F16" si="1">"'"&amp;B4&amp;"'"&amp;","</f>
+        <v>'Javascript',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>'#194973',</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>'CSS',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>'#5F9EA0',</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>'Node/Expresss',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="str">
+        <f>"'"&amp;C7&amp;"'"&amp;","</f>
+        <v>'#66CDAA',</v>
+      </c>
+      <c r="F7" t="str">
+        <f>"'"&amp;B7&amp;"'"&amp;","</f>
+        <v>'React',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>'#4B0082',</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>'SQL',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>'#D8BFD8',</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>'Mongo',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>'#FF8200',</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>'D3',</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>'#F09F0D',</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>'ChartsJS',</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>'#C73C1C',</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>'Recharts',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>'#708090',</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>'Project1',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>'#708090',</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>'Project2',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>'#708090',</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>'Project3',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="str">
+        <f>"'"&amp;C16&amp;"'"&amp;"]"</f>
+        <v>'#708090']</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>'Project4',</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>